<commit_message>
Track scaling of linear dominos
</commit_message>
<xml_diff>
--- a/qbenchmarks/analysis/games-analysis.xlsx
+++ b/qbenchmarks/analysis/games-analysis.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryant/repos/pgbdd/qbenchmarks/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07D61C9-F91A-6C4F-B35A-778E10CD14FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA24DB0-1949-C043-B478-FBD67DD88F19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="7360" windowWidth="26440" windowHeight="15440" xr2:uid="{583F3F6E-F0B6-1E45-809E-4DA5455BF68E}"/>
+    <workbookView xWindow="20180" yWindow="2840" windowWidth="31020" windowHeight="24320" activeTab="4" xr2:uid="{583F3F6E-F0B6-1E45-809E-4DA5455BF68E}"/>
   </bookViews>
   <sheets>
     <sheet name="NIM F4" sheetId="1" r:id="rId1"/>
     <sheet name="NIM T4" sheetId="2" r:id="rId2"/>
     <sheet name="LDOM A T" sheetId="3" r:id="rId3"/>
     <sheet name="LDOM B F" sheetId="4" r:id="rId4"/>
+    <sheet name="LDOM-BY5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
   <si>
     <t>N</t>
   </si>
@@ -81,15 +82,49 @@
   <si>
     <t>Trend LY</t>
   </si>
+  <si>
+    <t>SAT</t>
+  </si>
+  <si>
+    <t>REF</t>
+  </si>
+  <si>
+    <t>log C</t>
+  </si>
+  <si>
+    <t>Total Clauses</t>
+  </si>
+  <si>
+    <t>Input Clauses</t>
+  </si>
+  <si>
+    <t>Solve Time</t>
+  </si>
+  <si>
+    <t>log T</t>
+  </si>
+  <si>
+    <t>Qproof Time</t>
+  </si>
+  <si>
+    <t>Qrat Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,9 +150,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17C5056-3745-FB4B-B819-3956911D1C1A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -826,7 +862,7 @@
         <v>154972</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:D18" si="0">LOG(A3)</f>
+        <f t="shared" ref="C3:D14" si="0">LOG(A3)</f>
         <v>0.84509804001425681</v>
       </c>
       <c r="D3">
@@ -1419,7 +1455,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="E2" sqref="E2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2124,4 +2160,1421 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9015DD3F-8673-2F46-8038-D04A657C1A18}">
+  <dimension ref="A1:G94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>82</v>
+      </c>
+      <c r="C3">
+        <f>LOG(A3)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D3">
+        <f>LOG(B3)</f>
+        <v>1.9138138523837167</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" cm="1">
+        <f t="array" ref="F3">TREND(D$3:D$8,C$3:C$8,E3)</f>
+        <v>5.4616795897330483E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F4-F3</f>
+        <v>2.7094971370295666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>666</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D8" si="0">LOG(A4)</f>
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.823474229170301</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4">TREND(D$3:D$8,C$3:C$8,E4)</f>
+        <v>2.7641139329268971</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1725</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.2367890994092927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3880</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3.5888317255942073</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6637</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>3.821971817642043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>11166</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>4.0478976235144106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>81</v>
+      </c>
+      <c r="C11">
+        <f>LOG(A11)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D11">
+        <f>LOG(B11)</f>
+        <v>1.9084850188786497</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" cm="1">
+        <f t="array" ref="F11">TREND(D$11:D$18,C$11:C$18,E11)</f>
+        <v>6.2877729573054264E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <f>F12-F11</f>
+        <v>2.6995917555829618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>664</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C16" si="1">LOG(A12)</f>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D16" si="2">LOG(B12)</f>
+        <v>2.8221680793680175</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" cm="1">
+        <f t="array" ref="F12">TREND(D$11:D$18,C$11:C$18,E12)</f>
+        <v>2.7624694851560161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1728</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>3.2375437381428744</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>3885</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>3.5893910231369333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>6631</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>3.821579027912009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>11159</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>4.0476252775817834</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>24010</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:C18" si="3">LOG(A17)</f>
+        <v>1.6020599913279623</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D18" si="4">LOG(B17)</f>
+        <v>4.3803921600570277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18">
+        <v>43904</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="3"/>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="4"/>
+        <v>4.6425040896906387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5451</v>
+      </c>
+      <c r="C22">
+        <f>LOG(A22)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D22">
+        <f>LOG(B22)</f>
+        <v>3.7364761820276966</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" cm="1">
+        <f t="array" ref="F22">TREND(D$22:D$27,C$22:C$27,E22)</f>
+        <v>3.4850255563582344E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <f>F23-F22</f>
+        <v>5.3830750048722189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2">
+        <v>336886</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C27" si="5">LOG(A23)</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D27" si="6">LOG(B23)</f>
+        <v>5.5274829633435987</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" cm="1">
+        <f t="array" ref="F23">TREND(D$22:D$27,C$22:C$27,E23)</f>
+        <v>5.4179252604358012</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>15</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2235543</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="5"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="6"/>
+        <v>6.3493830278086669</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2">
+        <v>11293078</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="5"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="6"/>
+        <v>7.0528123277733075</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>33860508</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="5"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="6"/>
+        <v>7.5296934694238864</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2">
+        <v>93354759</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="5"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="6"/>
+        <v>7.9701364621325324</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>5937</v>
+      </c>
+      <c r="C30">
+        <f>LOG(A30)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D30">
+        <f>LOG(B30)</f>
+        <v>3.7735670489260587</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" cm="1">
+        <f t="array" ref="F30">TREND(D$30:D$37,C$30:C$37,E30)</f>
+        <v>0.91792037316895669</v>
+      </c>
+      <c r="G30" s="1">
+        <f>F31-F30</f>
+        <v>4.0532311867130435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>126127</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:C37" si="7">LOG(A31)</f>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:D37" si="8">LOG(B31)</f>
+        <v>5.1008080659214956</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" cm="1">
+        <f t="array" ref="F31">TREND(D$30:D$37,C$30:C$37,E31)</f>
+        <v>4.9711515598820002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>381593</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="7"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="8"/>
+        <v>5.5816003993411325</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>1232252</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="7"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="8"/>
+        <v>6.0906995317066634</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>3621470</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="7"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="8"/>
+        <v>6.5588848918870255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>7084367</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="7"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="8"/>
+        <v>6.8503010513811589</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>26150238</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="7"/>
+        <v>1.6020599913279623</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="8"/>
+        <v>7.4174756458463653</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>85077630</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="7"/>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="8"/>
+        <v>7.9298153832962974</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>0.1</v>
+      </c>
+      <c r="C41">
+        <f>LOG(A41)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D41">
+        <f>LOG(B41)</f>
+        <v>-1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" cm="1">
+        <f t="array" ref="F41">TREND(D$41:D$46,C$41:C$46,E41)</f>
+        <v>-4.8166791930635817</v>
+      </c>
+      <c r="G41" s="1">
+        <f>F42-F41</f>
+        <v>5.5236558887364682</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>6.41</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42:C46" si="9">LOG(A42)</f>
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42:D46" si="10">LOG(B42)</f>
+        <v>0.80685802951881747</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" cm="1">
+        <f t="array" ref="F42">TREND(D$41:D$46,C$41:C$46,E42)</f>
+        <v>0.70697669567288646</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>43.78</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="9"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="10"/>
+        <v>1.641275757231913</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>230.73</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="9"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="10"/>
+        <v>2.3631040660746354</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>25</v>
+      </c>
+      <c r="B45">
+        <v>790.98</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="9"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="10"/>
+        <v>2.898165502461711</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>30</v>
+      </c>
+      <c r="B46">
+        <v>2181.0300000000002</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="9"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="10"/>
+        <v>3.3386616393269128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>0.11</v>
+      </c>
+      <c r="C49">
+        <f>LOG(A49)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D49">
+        <f>LOG(B49)</f>
+        <v>-0.95860731484177497</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" cm="1">
+        <f t="array" ref="F49">TREND(D$49:D$56,C$49:C$56,E49)</f>
+        <v>-4.04847796790314</v>
+      </c>
+      <c r="G49" s="1">
+        <f>F50-F49</f>
+        <v>4.3130562504505088</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>2.38</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:C56" si="11">LOG(A50)</f>
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ref="D50:D56" si="12">LOG(B50)</f>
+        <v>0.37657695705651195</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" cm="1">
+        <f t="array" ref="F50">TREND(D$49:D$56,C$49:C$56,E50)</f>
+        <v>0.26457828254736881</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>7.67</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="11"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="12"/>
+        <v>0.88479536394898095</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>20</v>
+      </c>
+      <c r="B52">
+        <v>27.31</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="11"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="12"/>
+        <v>1.4363217001397333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>25</v>
+      </c>
+      <c r="B53">
+        <v>83.6</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="11"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="12"/>
+        <v>1.9222062774390163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>30</v>
+      </c>
+      <c r="B54">
+        <v>180.54</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="11"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="12"/>
+        <v>2.2565734381237244</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>40</v>
+      </c>
+      <c r="B55">
+        <v>762.6</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="11"/>
+        <v>1.6020599913279623</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="12"/>
+        <v>2.8822968009376519</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>50</v>
+      </c>
+      <c r="B56">
+        <v>2894.4</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="11"/>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="12"/>
+        <v>3.4615585495157384</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>0.08</v>
+      </c>
+      <c r="C60">
+        <f>LOG(A60)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D60">
+        <f>LOG(B60)</f>
+        <v>-1.0969100130080565</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" cm="1">
+        <f t="array" ref="F60">TREND(D$60:D$65,C$60:C$65,E60)</f>
+        <v>-5.2253515279105684</v>
+      </c>
+      <c r="G60" s="1">
+        <f>F61-F60</f>
+        <v>5.8616845957941663</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>5.04</v>
+      </c>
+      <c r="C61">
+        <f t="shared" ref="C61:C65" si="13">LOG(A61)</f>
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ref="D61:D65" si="14">LOG(B61)</f>
+        <v>0.70243053644552533</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" cm="1">
+        <f t="array" ref="F61">TREND(D$60:D$65,C$60:C$65,E61)</f>
+        <v>0.63633306788359789</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>15</v>
+      </c>
+      <c r="B62">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="13"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="14"/>
+        <v>1.5403294747908738</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>20</v>
+      </c>
+      <c r="B63">
+        <v>207.94</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="13"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="14"/>
+        <v>2.317938039636056</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>25</v>
+      </c>
+      <c r="B64">
+        <v>860.73</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="13"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="14"/>
+        <v>2.9348669401881544</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>30</v>
+      </c>
+      <c r="B65">
+        <v>3809.5</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="13"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="14"/>
+        <v>3.5808679779090302</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>0.08</v>
+      </c>
+      <c r="C68">
+        <f>LOG(A68)</f>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="D68">
+        <f>LOG(B68)</f>
+        <v>-1.0969100130080565</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" cm="1">
+        <f t="array" ref="F68">TREND(D$68:D$75,C$68:C$75,E68)</f>
+        <v>-4.196413250376172</v>
+      </c>
+      <c r="G68" s="1">
+        <f>F69-F68</f>
+        <v>4.3095282430756994</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>1.73</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ref="C69:C75" si="15">LOG(A69)</f>
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ref="D69:D75" si="16">LOG(B69)</f>
+        <v>0.2380461031287954</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" cm="1">
+        <f t="array" ref="F69">TREND(D$68:D$75,C$68:C$75,E69)</f>
+        <v>0.11311499269952741</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>15</v>
+      </c>
+      <c r="B70">
+        <v>5.41</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="15"/>
+        <v>1.1760912590556813</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="16"/>
+        <v>0.73319726510656946</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>20</v>
+      </c>
+      <c r="B71">
+        <v>17.86</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="15"/>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="16"/>
+        <v>1.2518814545525276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>25</v>
+      </c>
+      <c r="B72">
+        <v>56.64</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="15"/>
+        <v>1.3979400086720377</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="16"/>
+        <v>1.7531232446817127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>30</v>
+      </c>
+      <c r="B73">
+        <v>119.25</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="15"/>
+        <v>1.4771212547196624</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="16"/>
+        <v>2.0764583877121514</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>40</v>
+      </c>
+      <c r="B74">
+        <v>563.79999999999995</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="15"/>
+        <v>1.6020599913279623</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="16"/>
+        <v>2.7511250715355833</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>50</v>
+      </c>
+      <c r="B75">
+        <v>2161.6999999999998</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="15"/>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="16"/>
+        <v>3.3347954225567737</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.69896999999999998</v>
+      </c>
+      <c r="D79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E79" s="2">
+        <v>0</v>
+      </c>
+      <c r="F79" cm="1">
+        <f t="array" ref="F79">TREND(D$79:D$81,C$79:C$81,E79)</f>
+        <v>-4.8707301416209576</v>
+      </c>
+      <c r="G79" s="1">
+        <f>F80-F79</f>
+        <v>5.5860806996727694</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>10</v>
+      </c>
+      <c r="B80">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0.80685803</v>
+      </c>
+      <c r="E80" s="2">
+        <v>1</v>
+      </c>
+      <c r="F80" cm="1">
+        <f t="array" ref="F80">TREND(D$79:D$81,C$79:C$81,E80)</f>
+        <v>0.7153505580518118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <v>558.68399999999997</v>
+      </c>
+      <c r="C81" s="2">
+        <v>1.17609126</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1.6412757600000001</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0.69896999999999998</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1.9084850200000001</v>
+      </c>
+      <c r="E87" s="2">
+        <v>0</v>
+      </c>
+      <c r="F87" cm="1">
+        <f t="array" ref="F87">TREND(D$87:D$94,C$87:C$94,E87)</f>
+        <v>6.2877731247330981E-2</v>
+      </c>
+      <c r="G87" s="1">
+        <f>F88-F87</f>
+        <v>2.6995917569097565</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
+        <v>10</v>
+      </c>
+      <c r="B88">
+        <v>4.0259999999999998</v>
+      </c>
+      <c r="C88" s="2">
+        <v>1</v>
+      </c>
+      <c r="D88" s="2">
+        <v>2.82216808</v>
+      </c>
+      <c r="E88" s="2">
+        <v>1</v>
+      </c>
+      <c r="F88" cm="1">
+        <f t="array" ref="F88">TREND(D$87:D$94,C$87:C$94,E88)</f>
+        <v>2.7624694881570875</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
+        <v>15</v>
+      </c>
+      <c r="B89">
+        <v>19.978000000000002</v>
+      </c>
+      <c r="C89" s="2">
+        <v>1.17609126</v>
+      </c>
+      <c r="D89" s="2">
+        <v>3.23754374</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>20</v>
+      </c>
+      <c r="B90">
+        <v>68.694999999999993</v>
+      </c>
+      <c r="C90" s="2">
+        <v>1.3010299999999999</v>
+      </c>
+      <c r="D90" s="2">
+        <v>3.5893910199999999</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>25</v>
+      </c>
+      <c r="B91">
+        <v>127.229</v>
+      </c>
+      <c r="C91" s="2">
+        <v>1.3979400099999999</v>
+      </c>
+      <c r="D91" s="2">
+        <v>3.8215790300000001</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
+        <v>30</v>
+      </c>
+      <c r="B92">
+        <v>179.083</v>
+      </c>
+      <c r="C92" s="2">
+        <v>1.4771212499999999</v>
+      </c>
+      <c r="D92" s="2">
+        <v>4.0476252800000001</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
+        <v>40</v>
+      </c>
+      <c r="B93">
+        <v>2594.8910000000001</v>
+      </c>
+      <c r="C93" s="2">
+        <v>1.6020599900000001</v>
+      </c>
+      <c r="D93" s="2">
+        <v>4.3803921600000004</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>50</v>
+      </c>
+      <c r="B94">
+        <v>3342.8029999999999</v>
+      </c>
+      <c r="C94" s="2">
+        <v>1.6989700000000001</v>
+      </c>
+      <c r="D94" s="2">
+        <v>4.6425040900000001</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>